<commit_message>
Modificacion de plantilla generica
</commit_message>
<xml_diff>
--- a/Plantilla.xlsx
+++ b/Plantilla.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/318745c2dd4a0186/Facturacion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{CA471804-2467-4A5A-B715-C599CA217BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0CB431E-9B0C-4D8C-B6B8-F089C24ADB2F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D36AD29-1C8A-4734-8E9B-D8A5759B2348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E6D90268-911F-4225-9558-77472726293D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Cantidad</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>Total:</t>
-  </si>
-  <si>
-    <t>Tules</t>
   </si>
 </sst>
 </file>
@@ -866,7 +863,7 @@
   <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="90" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -884,9 +881,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
-        <v>10</v>
-      </c>
+      <c r="A1" s="31"/>
       <c r="B1" s="6"/>
       <c r="D1" s="27" t="s">
         <v>7</v>

</xml_diff>